<commit_message>
Added files sent by WRI 5/14/20
</commit_message>
<xml_diff>
--- a/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
+++ b/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\web-app\BpTPEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\India InputData 5-6-2020\web-app\BpTPEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1E666F-5E65-45D7-96CB-F35F25176F21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="14100"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BpTPEU-large" sheetId="2" r:id="rId2"/>
     <sheet name="BpTPEU-small" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Source:</t>
   </si>
@@ -32,35 +41,41 @@
     <t>BTU</t>
   </si>
   <si>
-    <t>none needed</t>
-  </si>
-  <si>
-    <t>For the U.S.:</t>
-  </si>
-  <si>
-    <t>large primary energy output unit</t>
-  </si>
-  <si>
-    <t>small primary energy output unit</t>
-  </si>
-  <si>
-    <t>The large primary energy output unit (used in totals graphs) is: quadrillion BTU</t>
-  </si>
-  <si>
-    <t>The small primary energy output unit (used in energy intensity per unit GDP graphs) is: thousand BTU</t>
-  </si>
-  <si>
     <t>BpTPEU BTU per Large Primary Energy Unit</t>
   </si>
   <si>
     <t>BpTPEU BTU per Small Primary Energy Unit</t>
+  </si>
+  <si>
+    <t>For India:</t>
+  </si>
+  <si>
+    <t>The large primary energy output unit (used in totals graphs) is: Petajoules</t>
+  </si>
+  <si>
+    <t>Google unit converter</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=btu+per+petajoule</t>
+  </si>
+  <si>
+    <t>One PJ</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=btu+per+kilojoule</t>
+  </si>
+  <si>
+    <t>The small primary energy output unit (used in energy intensity per unit GDP graphs) is: Megajoules</t>
+  </si>
+  <si>
+    <t>One MJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +87,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,19 +117,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -198,6 +227,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -233,6 +279,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -408,21 +471,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -430,11 +495,18 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -443,33 +515,39 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{4C805E71-826C-4130-895C-819426C4438A}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{5321D5F9-396D-45AA-8CD9-4C32A8CC087C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -477,24 +555,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>5</v>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
-        <f>10^15</f>
-        <v>1000000000000000</v>
+      <c r="B2" s="2">
+        <v>947800000000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
+      <c r="B10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -502,13 +579,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -516,24 +595,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>6</v>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <f>10^3</f>
-        <v>1000</v>
+      <c r="B2" s="3">
+        <v>947.81700000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
+      <c r="B10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>